<commit_message>
feat: book title 생성
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_Project\bookscramble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7EE7FFE-71E6-4A88-BE1A-4453D83BDA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3F6A2A-66FC-47D1-9004-8AE4D17873C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{185513D4-FECF-4B10-97B9-FDBD0DB77F8E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,13 +72,44 @@
   <si>
     <t>i</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Book Titles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +124,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFDEDE"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +154,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,57 +495,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B51406D-EF59-4A6A-B230-ECA32D66C201}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>